<commit_message>
Added ReadExcel & ReadExcelPOJO classes in java main utilities
</commit_message>
<xml_diff>
--- a/SampleSeleniumSetup/src/test/resources/TestData.xlsx
+++ b/SampleSeleniumSetup/src/test/resources/TestData.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0186E33A-5CD7-4938-8857-FFDA52384694}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3C002AA-FD32-4D2A-96B8-3059B697E66D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="330" windowWidth="14280" windowHeight="3240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestData!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -390,7 +390,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -414,6 +413,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="#32cd32" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -791,494 +791,490 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.26953125" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.26953125" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.81640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.1796875" style="2" customWidth="1" collapsed="1"/>
-    <col min="10" max="13" width="9.1796875" style="2"/>
-    <col min="14" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="1" max="1" width="30.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.54296875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.26953125" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.26953125" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="9.1796875" style="1"/>
+    <col min="14" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="D2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="D3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="D9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="D13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="D14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="D15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="D16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F20" s="3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ReadExcel with Filter Criteria complete.
</commit_message>
<xml_diff>
--- a/SampleSeleniumSetup/src/test/resources/TestData.xlsx
+++ b/SampleSeleniumSetup/src/test/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3C002AA-FD32-4D2A-96B8-3059B697E66D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F309A5FF-2008-470A-A4C9-AECE29CF2558}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="330" windowWidth="14280" windowHeight="3240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,51 +53,6 @@
     <t>Web</t>
   </si>
   <si>
-    <t>BsuinessModule1</t>
-  </si>
-  <si>
-    <t>BsuinessModule2</t>
-  </si>
-  <si>
-    <t>BsuinessModule3</t>
-  </si>
-  <si>
-    <t>BsuinessModule4</t>
-  </si>
-  <si>
-    <t>BsuinessModule5</t>
-  </si>
-  <si>
-    <t>BsuinessModule6</t>
-  </si>
-  <si>
-    <t>BsuinessModule7</t>
-  </si>
-  <si>
-    <t>BsuinessModule8</t>
-  </si>
-  <si>
-    <t>BsuinessModule9</t>
-  </si>
-  <si>
-    <t>BsuinessModule10</t>
-  </si>
-  <si>
-    <t>BsuinessModule11</t>
-  </si>
-  <si>
-    <t>BsuinessModule12</t>
-  </si>
-  <si>
-    <t>BsuinessModule13</t>
-  </si>
-  <si>
-    <t>BsuinessModule14</t>
-  </si>
-  <si>
-    <t>BsuinessModule15</t>
-  </si>
-  <si>
     <t>TestScript1</t>
   </si>
   <si>
@@ -231,6 +186,51 @@
   </si>
   <si>
     <t>LOB15</t>
+  </si>
+  <si>
+    <t>BusinessModule1</t>
+  </si>
+  <si>
+    <t>BusinessModule2</t>
+  </si>
+  <si>
+    <t>BusinessModule3</t>
+  </si>
+  <si>
+    <t>BusinessModule4</t>
+  </si>
+  <si>
+    <t>BusinessModule5</t>
+  </si>
+  <si>
+    <t>BusinessModule6</t>
+  </si>
+  <si>
+    <t>BusinessModule7</t>
+  </si>
+  <si>
+    <t>BusinessModule8</t>
+  </si>
+  <si>
+    <t>BusinessModule9</t>
+  </si>
+  <si>
+    <t>BusinessModule10</t>
+  </si>
+  <si>
+    <t>BusinessModule11</t>
+  </si>
+  <si>
+    <t>BusinessModule12</t>
+  </si>
+  <si>
+    <t>BusinessModule13</t>
+  </si>
+  <si>
+    <t>BusinessModule14</t>
+  </si>
+  <si>
+    <t>BusinessModule15</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,437 +844,437 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="12">
-        <v>0</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="12">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="12">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="12">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="12">
-        <v>0</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="H15" s="12">
-        <v>0</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="5">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>